<commit_message>
Actualizaciones guiones grado 8
Ajustes y solicitudes graficas 08_7, mapa y manuscrito final 08_13
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion07/CS_08_07_CO_Escaleta.xlsx
+++ b/fuentes/contenidos/grado08/guion07/CS_08_07_CO_Escaleta.xlsx
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$P$1:$P$284</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1083,6 +1083,63 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1117,63 +1174,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1513,94 +1513,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="65" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="63" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="F1" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="56" t="s">
+      <c r="H1" s="60" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="56" t="s">
+      <c r="I1" s="60" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="K1" s="69" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="48" t="s">
+      <c r="L1" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="71" t="s">
+      <c r="M1" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="71"/>
-      <c r="O1" s="63" t="s">
+      <c r="N1" s="62"/>
+      <c r="O1" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="63" t="s">
+      <c r="P1" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="65" t="s">
+      <c r="Q1" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="69" t="s">
+      <c r="R1" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="65" t="s">
+      <c r="S1" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="67" t="s">
+      <c r="T1" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="65" t="s">
+      <c r="U1" s="54" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="47"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="49"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="68"/>
       <c r="M2" s="40" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="70"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="68"/>
-      <c r="U2" s="66"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="55"/>
     </row>
     <row r="3" spans="1:21" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -1612,7 +1612,7 @@
       <c r="C3" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="72" t="s">
+      <c r="D3" s="47" t="s">
         <v>124</v>
       </c>
       <c r="E3" s="6"/>
@@ -1671,7 +1671,7 @@
       <c r="C4" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="73"/>
+      <c r="D4" s="48"/>
       <c r="E4" s="18" t="s">
         <v>129</v>
       </c>
@@ -1730,7 +1730,7 @@
       <c r="C5" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D5" s="73"/>
+      <c r="D5" s="48"/>
       <c r="E5" s="18" t="s">
         <v>134</v>
       </c>
@@ -1789,7 +1789,7 @@
       <c r="C6" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="73"/>
+      <c r="D6" s="48"/>
       <c r="E6" s="18" t="s">
         <v>138</v>
       </c>
@@ -1848,7 +1848,7 @@
       <c r="C7" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D7" s="74"/>
+      <c r="D7" s="49"/>
       <c r="E7" s="18" t="s">
         <v>142</v>
       </c>
@@ -1907,7 +1907,7 @@
       <c r="C8" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D8" s="60" t="s">
+      <c r="D8" s="44" t="s">
         <v>146</v>
       </c>
       <c r="E8" s="18" t="s">
@@ -1968,7 +1968,7 @@
       <c r="C9" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D9" s="61"/>
+      <c r="D9" s="45"/>
       <c r="E9" s="18" t="s">
         <v>153</v>
       </c>
@@ -2027,7 +2027,7 @@
       <c r="C10" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D10" s="61"/>
+      <c r="D10" s="45"/>
       <c r="E10" s="18" t="s">
         <v>156</v>
       </c>
@@ -2058,7 +2058,7 @@
       <c r="C11" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D11" s="61"/>
+      <c r="D11" s="45"/>
       <c r="E11" s="18" t="s">
         <v>157</v>
       </c>
@@ -2091,7 +2091,7 @@
       <c r="C12" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D12" s="61"/>
+      <c r="D12" s="45"/>
       <c r="E12" s="18"/>
       <c r="F12" s="13" t="s">
         <v>159</v>
@@ -2150,7 +2150,7 @@
       <c r="C13" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D13" s="61"/>
+      <c r="D13" s="45"/>
       <c r="E13" s="18" t="s">
         <v>163</v>
       </c>
@@ -2181,7 +2181,7 @@
       <c r="C14" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D14" s="62"/>
+      <c r="D14" s="46"/>
       <c r="E14" s="18" t="s">
         <v>142</v>
       </c>
@@ -2240,7 +2240,7 @@
       <c r="C15" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D15" s="60" t="s">
+      <c r="D15" s="44" t="s">
         <v>167</v>
       </c>
       <c r="E15" s="18" t="s">
@@ -2273,7 +2273,7 @@
       <c r="C16" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D16" s="61"/>
+      <c r="D16" s="45"/>
       <c r="E16" s="18" t="s">
         <v>169</v>
       </c>
@@ -2332,8 +2332,8 @@
       <c r="C17" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D17" s="61"/>
-      <c r="E17" s="58" t="s">
+      <c r="D17" s="45"/>
+      <c r="E17" s="50" t="s">
         <v>170</v>
       </c>
       <c r="F17" s="13"/>
@@ -2391,8 +2391,8 @@
       <c r="C18" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D18" s="61"/>
-      <c r="E18" s="59"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="51"/>
       <c r="F18" s="13"/>
       <c r="G18" s="19" t="s">
         <v>221</v>
@@ -2448,7 +2448,7 @@
       <c r="C19" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D19" s="62"/>
+      <c r="D19" s="46"/>
       <c r="E19" s="18" t="s">
         <v>142</v>
       </c>
@@ -2507,7 +2507,7 @@
       <c r="C20" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D20" s="60" t="s">
+      <c r="D20" s="44" t="s">
         <v>176</v>
       </c>
       <c r="E20" s="18"/>
@@ -2566,7 +2566,7 @@
       <c r="C21" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D21" s="61"/>
+      <c r="D21" s="45"/>
       <c r="E21" s="18" t="s">
         <v>179</v>
       </c>
@@ -2597,7 +2597,7 @@
       <c r="C22" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D22" s="61"/>
+      <c r="D22" s="45"/>
       <c r="E22" s="18" t="s">
         <v>180</v>
       </c>
@@ -2656,7 +2656,7 @@
       <c r="C23" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D23" s="61"/>
+      <c r="D23" s="45"/>
       <c r="E23" s="18" t="s">
         <v>184</v>
       </c>
@@ -2687,7 +2687,7 @@
       <c r="C24" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D24" s="61"/>
+      <c r="D24" s="45"/>
       <c r="E24" s="18" t="s">
         <v>185</v>
       </c>
@@ -2746,7 +2746,7 @@
       <c r="C25" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D25" s="62"/>
+      <c r="D25" s="46"/>
       <c r="E25" s="18" t="s">
         <v>142</v>
       </c>
@@ -2805,7 +2805,7 @@
       <c r="C26" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D26" s="60" t="s">
+      <c r="D26" s="44" t="s">
         <v>192</v>
       </c>
       <c r="E26" s="18" t="s">
@@ -2838,7 +2838,7 @@
       <c r="C27" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D27" s="61"/>
+      <c r="D27" s="45"/>
       <c r="E27" s="18" t="s">
         <v>224</v>
       </c>
@@ -2869,7 +2869,7 @@
       <c r="C28" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D28" s="61"/>
+      <c r="D28" s="45"/>
       <c r="E28" s="18" t="s">
         <v>194</v>
       </c>
@@ -2900,7 +2900,7 @@
       <c r="C29" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D29" s="62"/>
+      <c r="D29" s="46"/>
       <c r="E29" s="18" t="s">
         <v>142</v>
       </c>
@@ -2959,7 +2959,7 @@
       <c r="C30" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D30" s="60" t="s">
+      <c r="D30" s="44" t="s">
         <v>198</v>
       </c>
       <c r="E30" s="18"/>
@@ -3018,7 +3018,7 @@
       <c r="C31" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D31" s="62"/>
+      <c r="D31" s="46"/>
       <c r="E31" s="18"/>
       <c r="F31" s="13"/>
       <c r="G31" s="19" t="s">
@@ -3075,7 +3075,7 @@
       <c r="C32" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D32" s="60" t="s">
+      <c r="D32" s="44" t="s">
         <v>204</v>
       </c>
       <c r="E32" s="18"/>
@@ -3120,7 +3120,7 @@
       <c r="C33" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D33" s="61"/>
+      <c r="D33" s="45"/>
       <c r="E33" s="18"/>
       <c r="F33" s="13"/>
       <c r="G33" s="19" t="s">
@@ -3177,7 +3177,7 @@
       <c r="C34" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D34" s="62"/>
+      <c r="D34" s="46"/>
       <c r="E34" s="18"/>
       <c r="F34" s="13"/>
       <c r="G34" s="19" t="s">
@@ -4235,11 +4235,16 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="D3:D7"/>
-    <mergeCell ref="D8:D14"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="E17:E18"/>
     <mergeCell ref="D15:D19"/>
     <mergeCell ref="D20:D25"/>
@@ -4253,16 +4258,11 @@
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="D8:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>